<commit_message>
Plate Visualization Tool mostly functional
After restructuring (and restructuring and restructuring...) this will create an excel file from a verso txt file and worklist csv file that is a visualization of the verso file, but the barcode numbers are matched up to the PDSP numbers and also include which plates the compounds are in.

Need to add
* The file choosing menus
* Ability to process multiple verso files against 1 worklist (Most important)
* Ability to generate visualizations of the worklist (for both PRIM & SEC plates) (Good solution could be create one xlsx file that has tabs for each plate?)
* Ability to process a verso file on its own (not critically important as this situation is unlikely)
</commit_message>
<xml_diff>
--- a/Python_Scripts/Plate_Visualization_Tool/data_files/Map_Template.xlsx
+++ b/Python_Scripts/Plate_Visualization_Tool/data_files/Map_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kealbert\Documents\PDSP\Python_Scripts\Plate_Visualization_Tool\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207DEB58-0D93-40A8-9390-7AFC263D9BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02289188-488A-48C1-815C-B3A0F52AA93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,51 +17,17 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>A</t>
+    <t>Verso File Name:</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Layout Name:</t>
+    <t>Worklist File Name:</t>
   </si>
 </sst>
 </file>
@@ -71,15 +37,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -94,21 +55,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color indexed="8"/>
+      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -121,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -144,31 +103,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -478,238 +473,98 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="12.140625" style="3"/>
+    <col min="2" max="13" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="12.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8">
+        <v>7</v>
+      </c>
+      <c r="I3" s="8">
         <v>8</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="J3" s="8">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K3" s="8">
         <v>10</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L3" s="8">
         <v>11</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M3" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="4"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T11" s="5"/>
-    </row>
-    <row r="13" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:M1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="87" orientation="landscape" horizontalDpi="4294967293" verticalDpi="597" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="57" orientation="landscape" horizontalDpi="4294967293" verticalDpi="597" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="13" max="1048575" man="1"/>
   </colBreaks>
@@ -724,9 +579,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -738,8 +591,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>